<commit_message>
update sdk testcase and generate apidoc
</commit_message>
<xml_diff>
--- a/test/testcase/Wanchain RPC API Testcase.xlsx
+++ b/test/testcase/Wanchain RPC API Testcase.xlsx
@@ -794,30 +794,6 @@
   </si>
   <si>
     <t>method name wrong</t>
-  </si>
-  <si>
-    <t>Get the transmethod detail</t>
-  </si>
-  <si>
-    <t>Returns the number of transmethod in a given block by blockNumber or blockhash</t>
-  </si>
-  <si>
-    <t>Get the transmethod mined result</t>
-  </si>
-  <si>
-    <t>Return the receipt of a transmethod by transmethod hash</t>
-  </si>
-  <si>
-    <t>Return information of transmethod in a given block by blockNumber or blockhash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return information of transmethod via the specified address </t>
-  </si>
-  <si>
-    <t>Return information of transmethod via the specified address between the specified startblockno and endblockno</t>
-  </si>
-  <si>
-    <t>Send raw Transmethod</t>
   </si>
   <si>
     <t>Unrecognizable params</t>
@@ -6143,9 +6119,6 @@
 }</t>
   </si>
   <si>
-    <t>Create new message call transmethod or a contract creation for signed transaction</t>
-  </si>
-  <si>
     <t>{
   "jsonrpc": "2.0",
   "id": "user defined field",
@@ -6328,6 +6301,33 @@
   }]
 }</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create new message call transaction or a contract creation for signed transaction</t>
+  </si>
+  <si>
+    <t>Get the transaction detail</t>
+  </si>
+  <si>
+    <t>Returns the number of transaction in a given block by blockNumber or blockhash</t>
+  </si>
+  <si>
+    <t>Get the transaction mined result</t>
+  </si>
+  <si>
+    <t>Return the receipt of a transaction by transaction hash</t>
+  </si>
+  <si>
+    <t>Return information of transaction in a given block by blockNumber or blockhash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return information of transaction via the specified address </t>
+  </si>
+  <si>
+    <t>Return information of transaction via the specified address between the specified startblockno and endblockno</t>
+  </si>
+  <si>
+    <t>Send raw transaction</t>
   </si>
 </sst>
 </file>
@@ -7036,10 +7036,10 @@
   <dimension ref="A1:O116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -7079,7 +7079,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>13</v>
@@ -7090,10 +7090,10 @@
     </row>
     <row r="2" spans="1:15" ht="115.2">
       <c r="A2" s="4" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
@@ -7105,10 +7105,10 @@
         <v>17</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="6" t="s">
@@ -7133,10 +7133,10 @@
         <v>17</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
@@ -7161,10 +7161,10 @@
         <v>17</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
@@ -7192,14 +7192,14 @@
         <v>17</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="J5" s="4"/>
     </row>
@@ -7220,10 +7220,10 @@
         <v>17</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="13" t="s">
@@ -7248,10 +7248,10 @@
         <v>17</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -7274,10 +7274,10 @@
         <v>17</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -7300,10 +7300,10 @@
         <v>36</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -7326,10 +7326,10 @@
         <v>36</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -7337,13 +7337,13 @@
     </row>
     <row r="11" spans="1:15" ht="75.599999999999994" customHeight="1">
       <c r="A11" s="24" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>40</v>
@@ -7352,10 +7352,10 @@
         <v>36</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -7378,10 +7378,10 @@
         <v>36</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="6" t="s">
@@ -7397,7 +7397,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>47</v>
@@ -7406,10 +7406,10 @@
         <v>36</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="6" t="s">
@@ -7434,10 +7434,10 @@
         <v>36</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="6" t="s">
@@ -7462,10 +7462,10 @@
         <v>36</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="6" t="s">
@@ -7490,10 +7490,10 @@
         <v>17</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
@@ -7518,10 +7518,10 @@
         <v>17</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4" t="s">
@@ -7540,16 +7540,16 @@
         <v>61</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="6" t="s">
@@ -7568,16 +7568,16 @@
         <v>64</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="6" t="s">
@@ -7596,16 +7596,16 @@
         <v>64</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="6" t="s">
@@ -7624,16 +7624,16 @@
         <v>64</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4" t="s">
@@ -7652,16 +7652,16 @@
         <v>64</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="6" t="s">
@@ -7680,16 +7680,16 @@
         <v>71</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4" t="s">
@@ -7708,16 +7708,16 @@
         <v>71</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4" t="s">
@@ -7733,19 +7733,19 @@
         <v>42</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="6" t="s">
@@ -7764,16 +7764,16 @@
         <v>71</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4" t="s">
@@ -7792,16 +7792,16 @@
         <v>71</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4" t="s">
@@ -7826,10 +7826,10 @@
         <v>17</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="6" t="s">
@@ -7854,10 +7854,10 @@
         <v>17</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="6" t="s">
@@ -7882,10 +7882,10 @@
         <v>36</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="6" t="s">
@@ -7910,10 +7910,10 @@
         <v>17</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="6" t="s">
@@ -7938,10 +7938,10 @@
         <v>17</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="H32" s="4"/>
       <c r="I32" s="4" t="s">
@@ -7966,10 +7966,10 @@
         <v>17</v>
       </c>
       <c r="F33" s="25" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="G33" s="25" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="6" t="s">
@@ -7994,10 +7994,10 @@
         <v>17</v>
       </c>
       <c r="F34" s="25" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="G34" s="25" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
@@ -8016,16 +8016,16 @@
         <v>99</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>241</v>
+        <v>455</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F35" s="25" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="G35" s="25" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="6" t="s">
@@ -8050,10 +8050,10 @@
         <v>36</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="G36" s="25" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="6" t="s">
@@ -8078,10 +8078,10 @@
         <v>36</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="G37" s="25" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="6" t="s">
@@ -8097,19 +8097,19 @@
         <v>42</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>242</v>
+        <v>456</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="G38" s="25" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="6" t="s">
@@ -8125,19 +8125,19 @@
         <v>42</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>242</v>
+        <v>456</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="G39" s="25" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="6" t="s">
@@ -8153,19 +8153,19 @@
         <v>42</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>243</v>
+        <v>457</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="G40" s="25" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="6" t="s">
@@ -8181,19 +8181,19 @@
         <v>42</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>243</v>
+        <v>457</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F41" s="25" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="G41" s="25" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="6" t="s">
@@ -8209,19 +8209,19 @@
         <v>42</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>244</v>
+        <v>458</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="G42" s="25" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="6" t="s">
@@ -8237,19 +8237,19 @@
         <v>42</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>244</v>
+        <v>458</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="G43" s="25" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="6" t="s">
@@ -8274,10 +8274,10 @@
         <v>17</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="G44" s="25" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="4" t="s">
@@ -8302,10 +8302,10 @@
         <v>17</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="G45" s="25" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="H45" s="4"/>
       <c r="I45" s="6" t="s">
@@ -8324,16 +8324,16 @@
         <v>120</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>245</v>
+        <v>459</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F46" s="25" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="G46" s="25" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="6" t="s">
@@ -8352,16 +8352,16 @@
         <v>120</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>245</v>
+        <v>459</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F47" s="25" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="G47" s="25" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="6" t="s">
@@ -8380,16 +8380,16 @@
         <v>123</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>246</v>
+        <v>460</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="G48" s="25" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="6" t="s">
@@ -8408,16 +8408,16 @@
         <v>125</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>247</v>
+        <v>461</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F49" s="25" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="G49" s="25" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="H49" s="4"/>
       <c r="I49" s="6" t="s">
@@ -8442,10 +8442,10 @@
         <v>36</v>
       </c>
       <c r="F50" s="25" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="G50" s="25" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4" t="s">
@@ -8470,10 +8470,10 @@
         <v>17</v>
       </c>
       <c r="F51" s="25" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="G51" s="25" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="H51" s="4"/>
       <c r="I51" s="4" t="s">
@@ -8498,10 +8498,10 @@
         <v>17</v>
       </c>
       <c r="F52" s="25" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="G52" s="25" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="H52" s="4"/>
       <c r="I52" s="4" t="s">
@@ -8526,10 +8526,10 @@
         <v>17</v>
       </c>
       <c r="F53" s="25" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="G53" s="25" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="H53" s="4"/>
       <c r="I53" s="4" t="s">
@@ -8554,10 +8554,10 @@
         <v>17</v>
       </c>
       <c r="F54" s="25" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="G54" s="25" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="H54" s="4"/>
       <c r="I54" s="4" t="s">
@@ -8582,10 +8582,10 @@
         <v>17</v>
       </c>
       <c r="F55" s="25" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="G55" s="25" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="H55" s="4"/>
       <c r="I55" s="4" t="s">
@@ -8610,10 +8610,10 @@
         <v>17</v>
       </c>
       <c r="F56" s="25" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="G56" s="25" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="H56" s="4"/>
       <c r="I56" s="4" t="s">
@@ -8638,10 +8638,10 @@
         <v>17</v>
       </c>
       <c r="F57" s="25" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="G57" s="25" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="H57" s="4"/>
       <c r="I57" s="4" t="s">
@@ -8666,10 +8666,10 @@
         <v>17</v>
       </c>
       <c r="F58" s="25" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="G58" s="25" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="H58" s="4"/>
       <c r="I58" s="4" t="s">
@@ -8694,10 +8694,10 @@
         <v>17</v>
       </c>
       <c r="F59" s="25" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="G59" s="25" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="H59" s="4"/>
       <c r="I59" s="4" t="s">
@@ -8722,10 +8722,10 @@
         <v>17</v>
       </c>
       <c r="F60" s="25" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="G60" s="25" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="H60" s="4"/>
       <c r="I60" s="4" t="s">
@@ -8750,10 +8750,10 @@
         <v>17</v>
       </c>
       <c r="F61" s="25" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="G61" s="25" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="4" t="s">
@@ -8778,10 +8778,10 @@
         <v>17</v>
       </c>
       <c r="F62" s="25" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="G62" s="25" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="4" t="s">
@@ -8806,10 +8806,10 @@
         <v>17</v>
       </c>
       <c r="F63" s="25" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="G63" s="25" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="H63" s="4"/>
       <c r="I63" s="4" t="s">
@@ -8834,10 +8834,10 @@
         <v>17</v>
       </c>
       <c r="F64" s="25" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="G64" s="25" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="H64" s="4"/>
       <c r="I64" s="4" t="s">
@@ -8862,10 +8862,10 @@
         <v>36</v>
       </c>
       <c r="F65" s="25" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="G65" s="25" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="4" t="s">
@@ -8890,10 +8890,10 @@
         <v>17</v>
       </c>
       <c r="F66" s="25" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="G66" s="25" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="4" t="s">
@@ -8918,10 +8918,10 @@
         <v>17</v>
       </c>
       <c r="F67" s="25" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="G67" s="25" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="H67" s="4"/>
       <c r="I67" s="4" t="s">
@@ -8946,10 +8946,10 @@
         <v>17</v>
       </c>
       <c r="F68" s="25" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="G68" s="25" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="H68" s="4"/>
       <c r="I68" s="6" t="s">
@@ -8974,10 +8974,10 @@
         <v>17</v>
       </c>
       <c r="F69" s="25" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="G69" s="25" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="H69" s="4"/>
       <c r="I69" s="4" t="s">
@@ -9002,10 +9002,10 @@
         <v>17</v>
       </c>
       <c r="F70" s="25" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G70" s="25" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="H70" s="5"/>
       <c r="I70" s="6" t="s">
@@ -9030,10 +9030,10 @@
         <v>17</v>
       </c>
       <c r="F71" s="25" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G71" s="25" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="H71" s="4"/>
       <c r="I71" s="4" t="s">
@@ -9058,10 +9058,10 @@
         <v>17</v>
       </c>
       <c r="F72" s="25" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G72" s="25" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="H72" s="4"/>
       <c r="I72" s="4" t="s">
@@ -9086,10 +9086,10 @@
         <v>17</v>
       </c>
       <c r="F73" s="25" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="G73" s="25" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="H73" s="4"/>
       <c r="I73" s="4" t="s">
@@ -9114,10 +9114,10 @@
         <v>17</v>
       </c>
       <c r="F74" s="25" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="G74" s="25" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="H74" s="4"/>
       <c r="I74" s="4" t="s">
@@ -9136,16 +9136,16 @@
         <v>99</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>241</v>
+        <v>455</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F75" s="25" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="G75" s="25" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="H75" s="4"/>
       <c r="I75" s="4" t="s">
@@ -9170,10 +9170,10 @@
         <v>17</v>
       </c>
       <c r="F76" s="25" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="G76" s="25" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="H76" s="4"/>
       <c r="I76" s="4" t="s">
@@ -9198,10 +9198,10 @@
         <v>17</v>
       </c>
       <c r="F77" s="25" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="G77" s="25" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="H77" s="4"/>
       <c r="I77" s="4" t="s">
@@ -9217,19 +9217,19 @@
         <v>164</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>242</v>
+        <v>456</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F78" s="25" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="G78" s="25" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="H78" s="4"/>
       <c r="I78" s="4" t="s">
@@ -9245,19 +9245,19 @@
         <v>164</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>242</v>
+        <v>456</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F79" s="25" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="G79" s="25" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="H79" s="4"/>
       <c r="I79" s="4" t="s">
@@ -9273,19 +9273,19 @@
         <v>164</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>243</v>
+        <v>457</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F80" s="25" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="G80" s="25" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="H80" s="4"/>
       <c r="I80" s="6" t="s">
@@ -9301,19 +9301,19 @@
         <v>164</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>243</v>
+        <v>457</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F81" s="25" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="G81" s="25" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="4" t="s">
@@ -9329,19 +9329,19 @@
         <v>164</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>244</v>
+        <v>458</v>
       </c>
       <c r="E82" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F82" s="25" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="G82" s="25" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="6" t="s">
@@ -9357,19 +9357,19 @@
         <v>164</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>244</v>
+        <v>458</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F83" s="25" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="G83" s="25" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="H83" s="4"/>
       <c r="I83" s="4" t="s">
@@ -9388,16 +9388,16 @@
         <v>120</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>245</v>
+        <v>459</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F84" s="25" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="G84" s="25" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="4" t="s">
@@ -9416,16 +9416,16 @@
         <v>120</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>245</v>
+        <v>459</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F85" s="25" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="G85" s="25" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="4" t="s">
@@ -9444,16 +9444,16 @@
         <v>123</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>246</v>
+        <v>460</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F86" s="25" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="G86" s="25" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="H86" s="4"/>
       <c r="I86" s="4" t="s">
@@ -9472,16 +9472,16 @@
         <v>125</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>247</v>
+        <v>461</v>
       </c>
       <c r="E87" s="13" t="s">
         <v>17</v>
       </c>
       <c r="F87" s="26" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="G87" s="26" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="H87" s="13"/>
       <c r="I87" s="13" t="s">
@@ -9506,10 +9506,10 @@
         <v>17</v>
       </c>
       <c r="F88" s="25" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="G88" s="25" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="H88" s="4"/>
       <c r="I88" s="6" t="s">
@@ -9534,10 +9534,10 @@
         <v>17</v>
       </c>
       <c r="F89" s="25" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="G89" s="25" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="H89" s="4"/>
       <c r="I89" s="6" t="s">
@@ -9559,13 +9559,13 @@
         <v>128</v>
       </c>
       <c r="E90" s="24" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="F90" s="25" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="G90" s="25" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="H90" s="4"/>
       <c r="I90" s="4" t="s">
@@ -9590,10 +9590,10 @@
         <v>17</v>
       </c>
       <c r="F91" s="26" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="G91" s="26" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="H91" s="13"/>
       <c r="I91" s="13" t="s">
@@ -9618,10 +9618,10 @@
         <v>17</v>
       </c>
       <c r="F92" s="25" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="G92" s="25" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="H92" s="4"/>
       <c r="I92" s="4" t="s">
@@ -9646,10 +9646,10 @@
         <v>17</v>
       </c>
       <c r="F93" s="25" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="G93" s="25" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="H93" s="4"/>
       <c r="I93" s="4" t="s">
@@ -9674,10 +9674,10 @@
         <v>17</v>
       </c>
       <c r="F94" s="25" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="G94" s="25" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="H94" s="4"/>
       <c r="I94" s="4" t="s">
@@ -9702,10 +9702,10 @@
         <v>17</v>
       </c>
       <c r="F95" s="25" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="G95" s="25" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="H95" s="4"/>
       <c r="I95" s="4" t="s">
@@ -9730,10 +9730,10 @@
         <v>17</v>
       </c>
       <c r="F96" s="25" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="G96" s="25" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="H96" s="4"/>
       <c r="I96" s="4" t="s">
@@ -9758,10 +9758,10 @@
         <v>17</v>
       </c>
       <c r="F97" s="25" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="G97" s="25" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="H97" s="4"/>
       <c r="I97" s="4" t="s">
@@ -9786,10 +9786,10 @@
         <v>17</v>
       </c>
       <c r="F98" s="25" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="G98" s="25" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="H98" s="4"/>
       <c r="I98" s="4" t="s">
@@ -9814,10 +9814,10 @@
         <v>17</v>
       </c>
       <c r="F99" s="25" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="G99" s="25" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="H99" s="4"/>
       <c r="I99" s="4" t="s">
@@ -9842,10 +9842,10 @@
         <v>17</v>
       </c>
       <c r="F100" s="25" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="G100" s="25" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="H100" s="4"/>
       <c r="I100" s="4" t="s">
@@ -9870,10 +9870,10 @@
         <v>17</v>
       </c>
       <c r="F101" s="25" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="G101" s="25" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="H101" s="4"/>
       <c r="I101" s="4" t="s">
@@ -9898,10 +9898,10 @@
         <v>17</v>
       </c>
       <c r="F102" s="25" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G102" s="25" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="H102" s="4"/>
       <c r="I102" s="4" t="s">
@@ -9926,10 +9926,10 @@
         <v>17</v>
       </c>
       <c r="F103" s="25" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G103" s="25" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="H103" s="4"/>
       <c r="I103" s="4" t="s">
@@ -9954,10 +9954,10 @@
         <v>17</v>
       </c>
       <c r="F104" s="25" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="G104" s="25" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="H104" s="4"/>
       <c r="I104" s="4" t="s">
@@ -9982,10 +9982,10 @@
         <v>17</v>
       </c>
       <c r="F105" s="25" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="G105" s="25" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="H105" s="4"/>
       <c r="I105" s="4" t="s">
@@ -10010,10 +10010,10 @@
         <v>17</v>
       </c>
       <c r="F106" s="25" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="G106" s="25" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="H106" s="4"/>
       <c r="I106" s="4" t="s">
@@ -10038,10 +10038,10 @@
         <v>17</v>
       </c>
       <c r="F107" s="25" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="G107" s="25" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="H107" s="4"/>
       <c r="I107" s="4" t="s">
@@ -10057,7 +10057,7 @@
         <v>209</v>
       </c>
       <c r="C108" s="17" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="D108" s="17" t="s">
         <v>47</v>
@@ -10066,10 +10066,10 @@
         <v>36</v>
       </c>
       <c r="F108" s="27" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="G108" s="27" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="H108" s="17"/>
       <c r="I108" s="17" t="s">
@@ -10085,7 +10085,7 @@
         <v>209</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>211</v>
@@ -10094,10 +10094,10 @@
         <v>36</v>
       </c>
       <c r="F109" s="25" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="G109" s="25" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="H109" s="4"/>
       <c r="I109" s="4" t="s">
@@ -10122,10 +10122,10 @@
         <v>36</v>
       </c>
       <c r="F110" s="28" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="G110" s="28" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="H110" s="18"/>
       <c r="I110" s="18" t="s">
@@ -10150,10 +10150,10 @@
         <v>17</v>
       </c>
       <c r="F111" s="25" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="G111" s="25" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="H111" s="4"/>
       <c r="I111" s="4" t="s">
@@ -10172,16 +10172,16 @@
         <v>89</v>
       </c>
       <c r="D112" s="20" t="s">
-        <v>248</v>
+        <v>462</v>
       </c>
       <c r="E112" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F112" s="28" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="G112" s="28" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="H112" s="18"/>
       <c r="I112" s="18" t="s">
@@ -10206,10 +10206,10 @@
         <v>36</v>
       </c>
       <c r="F113" s="25" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="G113" s="25" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="H113" s="4"/>
       <c r="I113" s="4" t="s">
@@ -10225,7 +10225,7 @@
         <v>209</v>
       </c>
       <c r="C114" s="19" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="D114" s="20" t="s">
         <v>221</v>
@@ -10234,10 +10234,10 @@
         <v>17</v>
       </c>
       <c r="F114" s="28" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="G114" s="28" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="H114" s="18"/>
       <c r="I114" s="18" t="s">
@@ -10253,7 +10253,7 @@
         <v>209</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>213</v>
@@ -10262,10 +10262,10 @@
         <v>36</v>
       </c>
       <c r="F115" s="25" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="G115" s="25" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="H115" s="4"/>
       <c r="I115" s="4" t="s">
@@ -10290,10 +10290,10 @@
         <v>17</v>
       </c>
       <c r="F116" s="25" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="G116" s="25" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="H116" s="4"/>
       <c r="I116" s="4" t="s">

</xml_diff>

<commit_message>
remove getTransaction; add option argument[format] for getTxInfo; update docmentation
</commit_message>
<xml_diff>
--- a/test/testcase/Wanchain RPC API Testcase.xlsx
+++ b/test/testcase/Wanchain RPC API Testcase.xlsx
@@ -5753,9 +5753,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>getTransaction</t>
-  </si>
-  <si>
     <t>getUTXO</t>
   </si>
   <si>
@@ -5770,18 +5767,6 @@
           "address": ["mtCotFuC1JP448Y3uhEbyPeP7UduYUn6Vb"]
     }
 }</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
- "jsonrpc": "2.0",
-        "id": "user defined field",
-        "method": "getTransaction",
-        "params": {
-          "chainType":"BTC",
-         "txHash":"7168a86c84eda0bbfb7ae553118b02983516e8a6c448dc4c0630d26299297f20"
-        }
-      }</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -6327,6 +6312,22 @@
   "id": "user defined field",
   "result": "180000000000"
 }</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "jsonrpc": "2.0",
+        "id": "user defined field",
+        "method": "getTxInfo",
+        "params": {
+          "chainType":"BTC","format":true
+         "txHash":"7168a86c84eda0bbfb7ae553118b02983516e8a6c448dc4c0630d26299297f20"
+        }
+      }</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>getTxInfo</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -6647,6 +6648,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -6704,7 +6773,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CAEACE"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -7036,10 +7105,10 @@
   <dimension ref="A1:O116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C114" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G65" sqref="G65"/>
+      <selection pane="bottomRight" activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -7633,7 +7702,7 @@
         <v>406</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4" t="s">
@@ -7733,7 +7802,7 @@
         <v>42</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>413</v>
@@ -7745,7 +7814,7 @@
         <v>408</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="6" t="s">
@@ -7904,7 +7973,7 @@
         <v>89</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>17</v>
@@ -7932,7 +8001,7 @@
         <v>89</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>17</v>
@@ -7960,7 +8029,7 @@
         <v>89</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>17</v>
@@ -7988,7 +8057,7 @@
         <v>89</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>17</v>
@@ -8016,7 +8085,7 @@
         <v>99</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>36</v>
@@ -8025,7 +8094,7 @@
         <v>259</v>
       </c>
       <c r="G35" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="6" t="s">
@@ -8053,7 +8122,7 @@
         <v>260</v>
       </c>
       <c r="G36" s="25" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="6" t="s">
@@ -8081,7 +8150,7 @@
         <v>261</v>
       </c>
       <c r="G37" s="25" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="6" t="s">
@@ -8100,7 +8169,7 @@
         <v>390</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>17</v>
@@ -8128,7 +8197,7 @@
         <v>390</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>36</v>
@@ -8156,7 +8225,7 @@
         <v>372</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>17</v>
@@ -8165,7 +8234,7 @@
         <v>373</v>
       </c>
       <c r="G40" s="25" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="6" t="s">
@@ -8184,7 +8253,7 @@
         <v>372</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>17</v>
@@ -8212,16 +8281,16 @@
         <v>385</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="G42" s="25" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="6" t="s">
@@ -8240,7 +8309,7 @@
         <v>385</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>17</v>
@@ -8274,10 +8343,10 @@
         <v>17</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="G44" s="25" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="4" t="s">
@@ -8296,7 +8365,7 @@
         <v>89</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>17</v>
@@ -8324,7 +8393,7 @@
         <v>120</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>36</v>
@@ -8333,7 +8402,7 @@
         <v>262</v>
       </c>
       <c r="G46" s="25" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="6" t="s">
@@ -8352,7 +8421,7 @@
         <v>120</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>36</v>
@@ -8361,7 +8430,7 @@
         <v>263</v>
       </c>
       <c r="G47" s="25" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="6" t="s">
@@ -8380,7 +8449,7 @@
         <v>123</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>36</v>
@@ -8389,7 +8458,7 @@
         <v>264</v>
       </c>
       <c r="G48" s="25" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="6" t="s">
@@ -8408,7 +8477,7 @@
         <v>125</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>36</v>
@@ -8417,7 +8486,7 @@
         <v>318</v>
       </c>
       <c r="G49" s="25" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H49" s="4"/>
       <c r="I49" s="6" t="s">
@@ -8445,7 +8514,7 @@
         <v>265</v>
       </c>
       <c r="G50" s="25" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4" t="s">
@@ -8865,7 +8934,7 @@
         <v>280</v>
       </c>
       <c r="G65" s="25" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="4" t="s">
@@ -9108,7 +9177,7 @@
         <v>89</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>17</v>
@@ -9136,7 +9205,7 @@
         <v>99</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>17</v>
@@ -9220,7 +9289,7 @@
         <v>390</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>17</v>
@@ -9248,7 +9317,7 @@
         <v>390</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>17</v>
@@ -9276,7 +9345,7 @@
         <v>372</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>36</v>
@@ -9285,7 +9354,7 @@
         <v>375</v>
       </c>
       <c r="G80" s="25" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="H80" s="4"/>
       <c r="I80" s="6" t="s">
@@ -9304,7 +9373,7 @@
         <v>372</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>17</v>
@@ -9332,7 +9401,7 @@
         <v>385</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E82" s="4" t="s">
         <v>36</v>
@@ -9341,7 +9410,7 @@
         <v>387</v>
       </c>
       <c r="G82" s="25" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="6" t="s">
@@ -9360,7 +9429,7 @@
         <v>385</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>17</v>
@@ -9388,7 +9457,7 @@
         <v>120</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>17</v>
@@ -9397,7 +9466,7 @@
         <v>292</v>
       </c>
       <c r="G84" s="25" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="4" t="s">
@@ -9416,7 +9485,7 @@
         <v>120</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>17</v>
@@ -9425,7 +9494,7 @@
         <v>293</v>
       </c>
       <c r="G85" s="25" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="4" t="s">
@@ -9444,7 +9513,7 @@
         <v>123</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>17</v>
@@ -9453,7 +9522,7 @@
         <v>294</v>
       </c>
       <c r="G86" s="25" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H86" s="4"/>
       <c r="I86" s="4" t="s">
@@ -9472,7 +9541,7 @@
         <v>125</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E87" s="13" t="s">
         <v>17</v>
@@ -9481,7 +9550,7 @@
         <v>295</v>
       </c>
       <c r="G87" s="26" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H87" s="13"/>
       <c r="I87" s="13" t="s">
@@ -9506,10 +9575,10 @@
         <v>17</v>
       </c>
       <c r="F88" s="25" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="G88" s="25" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H88" s="4"/>
       <c r="I88" s="6" t="s">
@@ -9528,7 +9597,7 @@
         <v>89</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>17</v>
@@ -10069,7 +10138,7 @@
         <v>363</v>
       </c>
       <c r="G108" s="27" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H108" s="17"/>
       <c r="I108" s="17" t="s">
@@ -10085,7 +10154,7 @@
         <v>209</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>211</v>
@@ -10094,10 +10163,10 @@
         <v>36</v>
       </c>
       <c r="F109" s="25" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G109" s="25" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="H109" s="4"/>
       <c r="I109" s="4" t="s">
@@ -10172,7 +10241,7 @@
         <v>89</v>
       </c>
       <c r="D112" s="20" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E112" s="18" t="s">
         <v>17</v>
@@ -10225,7 +10294,7 @@
         <v>209</v>
       </c>
       <c r="C114" s="19" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D114" s="20" t="s">
         <v>221</v>
@@ -10234,7 +10303,7 @@
         <v>17</v>
       </c>
       <c r="F114" s="28" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G114" s="28" t="s">
         <v>401</v>
@@ -10253,7 +10322,7 @@
         <v>209</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>426</v>
+        <v>462</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>213</v>
@@ -10262,7 +10331,7 @@
         <v>36</v>
       </c>
       <c r="F115" s="25" t="s">
-        <v>429</v>
+        <v>461</v>
       </c>
       <c r="G115" s="25" t="s">
         <v>357</v>

</xml_diff>

<commit_message>
update doc, change erc20 api to token api
</commit_message>
<xml_diff>
--- a/test/testcase/Wanchain RPC API Testcase.xlsx
+++ b/test/testcase/Wanchain RPC API Testcase.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13320" activeTab="1"/>
@@ -15,7 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">testcases!$A$1:$O$44</definedName>
     <definedName name="Z_039CC8E6_E3A9_41D2_8462_8CF34EAE656B_.wvu.FilterData" localSheetId="1" hidden="1">testcases!$A$1:$O$44</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -106,27 +106,18 @@
     <t>TC0006</t>
   </si>
   <si>
-    <t>getErc20Info</t>
-  </si>
-  <si>
     <t>Get the info of ERC20 contract, like symbol and decimals</t>
   </si>
   <si>
     <t>TC0007</t>
   </si>
   <si>
-    <t>getMultiErc20Info</t>
-  </si>
-  <si>
     <t>Get the infos of muti ERC20 contracts, like symbol and decimals</t>
   </si>
   <si>
     <t>TC0008</t>
   </si>
   <si>
-    <t>getErc20Allowance</t>
-  </si>
-  <si>
     <t>Get the erc20 allowance for one specific account on one  contract for one specific spender account</t>
   </si>
   <si>
@@ -134,9 +125,6 @@
   </si>
   <si>
     <t>TC0009</t>
-  </si>
-  <si>
-    <t>getRegErc20Tokens</t>
   </si>
   <si>
     <t>Get the detail info of registered contract for Erc20_crosschain, like address, ratio, etc</t>
@@ -820,55 +808,6 @@
   "id": "user defined field",
   "method": "getGasPrice",
   "params": {
-  }
-}</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-  "jsonrpc": "2.0",
-  "id": "user defined field",
-  "method": "getErc20Info",
-  "params": {
-    "chainType":"ETH",
-    "tokenScAddr":"0xc5bc855056d99ef4bda0a4ae937065315e2ae11a"
-  }
-}</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-  "jsonrpc": "2.0",
-  "id": "user defined field",
-  "method": "getMultiErc20Info",
-  "params": {
-    "chainType":"ETH",
-    "tokenScAddrArray":["0xc5bc855056d99ef4bda0a4ae937065315e2ae11a","0x7017500899433272b4088afe34c04d742d0ce7df" ]
-  }
-}</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-  "jsonrpc": "2.0",
-  "id": "user defined field",
-  "method": "getErc20Allowance",
-  "params": {
-    "chainType":"ETH",
-    "tokenScAddr":"0xc5bc855056d99ef4bda0a4ae937065315e2ae11a",
-    "ownerAddr":"0xc27ecd85faa4ae80bf5e28daf91b605db7be1ba8",
-    "spenderAddr":"0xcdc96fea7e2a6ce584df5dc22d9211e53a5b18b1"
-  }
-}</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-  "jsonrpc": "2.0",
-  "id": "user defined field",
-  "method": "getRegErc20Tokens",
-  "params": {
-    "crossChain":"ETH"
   }
 }</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -5437,23 +5376,8 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>{
-  "jsonrpc": "2.0",
-  "id": "user defined field",
-  "method": "getErc20StoremanGroups",
-  "params": {
-    "crossChain":"ETH",
-    "tokenScAddr":"0xc5bc855056d99ef4bda0a4ae937065315e2ae11a"
-  }
-}</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>TC0010</t>
     <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>getErc20StoremanGroups</t>
   </si>
   <si>
     <t>{
@@ -6329,6 +6253,77 @@
         }
       }</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>getTokenStoremanGroups</t>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "user defined field",
+  "method": "getTokenStoremanGroups",
+  "params": {
+    "crossChain":"ETH",
+    "tokenScAddr":"0xc5bc855056d99ef4bda0a4ae937065315e2ae11a"
+  }
+}</t>
+  </si>
+  <si>
+    <t>getRegTokens</t>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "user defined field",
+  "method": "getRegTokens",
+  "params": {
+    "crossChain":"ETH"
+  }
+}</t>
+  </si>
+  <si>
+    <t>getTokenAllowance</t>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "user defined field",
+  "method": "getTokenAllowance",
+  "params": {
+    "chainType":"ETH",
+    "tokenScAddr":"0xc5bc855056d99ef4bda0a4ae937065315e2ae11a",
+    "ownerAddr":"0xc27ecd85faa4ae80bf5e28daf91b605db7be1ba8",
+    "spenderAddr":"0xcdc96fea7e2a6ce584df5dc22d9211e53a5b18b1"
+  }
+}</t>
+  </si>
+  <si>
+    <t>getTokenInfo</t>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "user defined field",
+  "method": "getTokenInfo",
+  "params": {
+    "chainType":"ETH",
+    "tokenScAddr":"0xc5bc855056d99ef4bda0a4ae937065315e2ae11a"
+  }
+}</t>
+  </si>
+  <si>
+    <t>getMultiTokenInfo</t>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "user defined field",
+  "method": "getMultiTokenInfo",
+  "params": {
+    "chainType":"ETH",
+    "tokenScAddrArray":["0xc5bc855056d99ef4bda0a4ae937065315e2ae11a","0x7017500899433272b4088afe34c04d742d0ce7df" ]
+  }
+}</t>
   </si>
 </sst>
 </file>
@@ -7037,10 +7032,10 @@
   <dimension ref="A1:O116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C114" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F115" sqref="F115"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -7080,7 +7075,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>13</v>
@@ -7091,10 +7086,10 @@
     </row>
     <row r="2" spans="1:15" ht="115.2">
       <c r="A2" s="4" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
@@ -7106,10 +7101,10 @@
         <v>17</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="6" t="s">
@@ -7134,14 +7129,14 @@
         <v>17</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="J3" s="4"/>
     </row>
@@ -7162,14 +7157,14 @@
         <v>17</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="J4" s="4"/>
       <c r="O4" t="s">
@@ -7193,14 +7188,14 @@
         <v>17</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="J5" s="4"/>
     </row>
@@ -7221,10 +7216,10 @@
         <v>17</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="13" t="s">
@@ -7240,19 +7235,19 @@
         <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>245</v>
+        <v>460</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -7260,25 +7255,25 @@
     </row>
     <row r="8" spans="1:15" ht="75.599999999999994" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>31</v>
+        <v>461</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>246</v>
+        <v>462</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -7286,25 +7281,25 @@
     </row>
     <row r="9" spans="1:15" ht="75.599999999999994" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>34</v>
+        <v>457</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>247</v>
+        <v>458</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -7312,25 +7307,25 @@
     </row>
     <row r="10" spans="1:15" ht="75.599999999999994" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>38</v>
+        <v>455</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>248</v>
+        <v>456</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -7338,25 +7333,25 @@
     </row>
     <row r="11" spans="1:15" ht="75.599999999999994" customHeight="1">
       <c r="A11" s="24" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>404</v>
+        <v>453</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>402</v>
+        <v>454</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -7364,1494 +7359,1494 @@
     </row>
     <row r="12" spans="1:15" ht="75.599999999999994" customHeight="1">
       <c r="A12" s="12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:15" ht="230.4">
       <c r="A13" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:15" ht="144">
       <c r="A14" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:15" ht="129.6">
       <c r="A15" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:15" ht="158.4">
       <c r="A16" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="144">
       <c r="A17" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="172.8">
       <c r="A18" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" ht="172.8">
       <c r="A19" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10" ht="158.4">
       <c r="A20" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" ht="172.8">
       <c r="A21" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" ht="158.4">
       <c r="A22" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" ht="187.2">
       <c r="A23" s="12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" ht="172.8">
       <c r="A24" s="12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:10" ht="187.2">
       <c r="A25" s="12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J25" s="4"/>
     </row>
     <row r="26" spans="1:10" ht="172.8">
       <c r="A26" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" ht="187.2">
       <c r="A27" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:10" ht="158.4">
       <c r="A28" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:10" ht="158.4">
       <c r="A29" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J29" s="15"/>
     </row>
     <row r="30" spans="1:10" ht="129.6">
       <c r="A30" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" ht="201.6">
       <c r="A31" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:10" ht="201.6">
       <c r="A32" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="H32" s="4"/>
       <c r="I32" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" ht="216">
       <c r="A33" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F33" s="25" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="G33" s="25" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J33" s="6"/>
     </row>
     <row r="34" spans="1:10" ht="216">
       <c r="A34" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F34" s="25" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="G34" s="25" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:10" ht="100.2" customHeight="1">
       <c r="A35" s="12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F35" s="25" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="G35" s="25" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="147" customHeight="1">
       <c r="A36" s="12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="G36" s="25" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J36" s="6"/>
     </row>
     <row r="37" spans="1:10" ht="147" customHeight="1">
       <c r="A37" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="G37" s="25" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J37" s="6"/>
     </row>
     <row r="38" spans="1:10" ht="147" customHeight="1">
       <c r="A38" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="G38" s="25" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J38" s="16"/>
     </row>
     <row r="39" spans="1:10" ht="147" customHeight="1">
       <c r="A39" s="12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="G39" s="25" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J39" s="16"/>
     </row>
     <row r="40" spans="1:10" ht="127.2" customHeight="1">
       <c r="A40" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="G40" s="25" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J40" s="6"/>
     </row>
     <row r="41" spans="1:10" ht="172.8">
       <c r="A41" s="12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F41" s="25" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="G41" s="25" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="245.4" customHeight="1">
       <c r="A42" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
       <c r="G42" s="25" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="172.8">
       <c r="A43" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="G43" s="25" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J43" s="6"/>
     </row>
     <row r="44" spans="1:10" ht="83.4" customHeight="1">
       <c r="A44" s="12" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="G44" s="25" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J44" s="4"/>
     </row>
     <row r="45" spans="1:10" ht="201.6">
       <c r="A45" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="G45" s="25" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="H45" s="4"/>
       <c r="I45" s="6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J45" s="4"/>
     </row>
     <row r="46" spans="1:10" ht="302.39999999999998">
       <c r="A46" s="12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F46" s="25" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="G46" s="25" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J46" s="16"/>
     </row>
     <row r="47" spans="1:10" ht="302.39999999999998">
       <c r="A47" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F47" s="25" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="G47" s="25" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J47" s="16"/>
     </row>
     <row r="48" spans="1:10" ht="409.6">
       <c r="A48" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="G48" s="25" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J48" s="16"/>
     </row>
     <row r="49" spans="1:10" ht="409.6">
       <c r="A49" s="12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F49" s="25" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="G49" s="25" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="H49" s="4"/>
       <c r="I49" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J49" s="16"/>
     </row>
     <row r="50" spans="1:10" ht="127.95" customHeight="1">
       <c r="A50" s="12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F50" s="25" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="G50" s="25" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J50" s="4"/>
     </row>
     <row r="51" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A51" s="12" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F51" s="25" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="G51" s="25" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="H51" s="4"/>
       <c r="I51" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J51" s="4"/>
     </row>
     <row r="52" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A52" s="12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F52" s="25" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="G52" s="25" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="H52" s="4"/>
       <c r="I52" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J52" s="4"/>
     </row>
     <row r="53" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A53" s="12" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F53" s="25" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="G53" s="25" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="H53" s="4"/>
       <c r="I53" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J53" s="4"/>
     </row>
     <row r="54" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A54" s="12" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F54" s="25" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="G54" s="25" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="H54" s="4"/>
       <c r="I54" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J54" s="4"/>
     </row>
     <row r="55" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A55" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F55" s="25" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="G55" s="25" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="H55" s="4"/>
       <c r="I55" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J55" s="4"/>
     </row>
     <row r="56" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A56" s="12" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F56" s="25" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="G56" s="25" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="H56" s="4"/>
       <c r="I56" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J56" s="4"/>
     </row>
     <row r="57" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A57" s="12" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F57" s="25" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="G57" s="25" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="H57" s="4"/>
       <c r="I57" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J57" s="4"/>
     </row>
     <row r="58" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A58" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F58" s="25" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="G58" s="25" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="H58" s="4"/>
       <c r="I58" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J58" s="4"/>
     </row>
     <row r="59" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A59" s="12" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F59" s="25" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="G59" s="25" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="H59" s="4"/>
       <c r="I59" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J59" s="4"/>
     </row>
     <row r="60" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A60" s="12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F60" s="25" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="G60" s="25" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="H60" s="4"/>
       <c r="I60" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J60" s="4"/>
     </row>
     <row r="61" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A61" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F61" s="25" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="G61" s="25" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J61" s="4"/>
     </row>
     <row r="62" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A62" s="12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F62" s="25" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="G62" s="25" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J62" s="4"/>
     </row>
     <row r="63" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A63" s="12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F63" s="25" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="G63" s="25" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="H63" s="4"/>
       <c r="I63" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J63" s="4"/>
     </row>
     <row r="64" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A64" s="12" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F64" s="25" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="G64" s="25" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="H64" s="4"/>
       <c r="I64" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="J64" s="4"/>
     </row>
     <row r="65" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A65" s="12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>24</v>
@@ -8860,726 +8855,726 @@
         <v>25</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F65" s="25" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="G65" s="25" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J65" s="4"/>
     </row>
     <row r="66" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A66" s="12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F66" s="25" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="G66" s="25" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J66" s="15"/>
     </row>
     <row r="67" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A67" s="12" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F67" s="25" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="G67" s="25" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="H67" s="4"/>
       <c r="I67" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="J67" s="15"/>
     </row>
     <row r="68" spans="1:10" ht="144">
       <c r="A68" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F68" s="25" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="G68" s="25" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="H68" s="4"/>
       <c r="I68" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J68" s="4"/>
     </row>
     <row r="69" spans="1:10" ht="158.4">
       <c r="A69" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F69" s="25" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="G69" s="25" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="H69" s="4"/>
       <c r="I69" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J69" s="4"/>
     </row>
     <row r="70" spans="1:10" ht="158.4">
       <c r="A70" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F70" s="25" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="G70" s="25" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="H70" s="5"/>
       <c r="I70" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J70" s="5"/>
     </row>
     <row r="71" spans="1:10" ht="144">
       <c r="A71" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F71" s="25" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="G71" s="25" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="H71" s="4"/>
       <c r="I71" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J71" s="4"/>
     </row>
     <row r="72" spans="1:10" ht="144">
       <c r="A72" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F72" s="25" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="G72" s="25" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="H72" s="4"/>
       <c r="I72" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J72" s="4"/>
     </row>
     <row r="73" spans="1:10" ht="144">
       <c r="A73" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F73" s="25" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="G73" s="25" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="H73" s="4"/>
       <c r="I73" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J73" s="15"/>
     </row>
     <row r="74" spans="1:10" ht="201.6">
       <c r="A74" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F74" s="25" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="G74" s="25" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="H74" s="4"/>
       <c r="I74" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="J74" s="4"/>
     </row>
     <row r="75" spans="1:10" ht="144">
       <c r="A75" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F75" s="25" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="G75" s="25" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="H75" s="4"/>
       <c r="I75" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J75" s="4"/>
     </row>
     <row r="76" spans="1:10" ht="125.4" customHeight="1">
       <c r="A76" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F76" s="25" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="G76" s="25" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="H76" s="4"/>
       <c r="I76" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J76" s="4"/>
     </row>
     <row r="77" spans="1:10" ht="125.4" customHeight="1">
       <c r="A77" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F77" s="25" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="G77" s="25" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="H77" s="4"/>
       <c r="I77" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J77" s="4"/>
     </row>
     <row r="78" spans="1:10" ht="129.6">
       <c r="A78" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F78" s="25" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="G78" s="25" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="H78" s="4"/>
       <c r="I78" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J78" s="15"/>
     </row>
     <row r="79" spans="1:10" ht="158.4">
       <c r="A79" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F79" s="25" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="G79" s="25" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="H79" s="4"/>
       <c r="I79" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J79" s="15"/>
     </row>
     <row r="80" spans="1:10" ht="97.2" customHeight="1">
       <c r="A80" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F80" s="25" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="G80" s="25" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="H80" s="4"/>
       <c r="I80" s="6" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J80" s="6"/>
     </row>
     <row r="81" spans="1:10" ht="172.8">
       <c r="A81" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F81" s="25" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="G81" s="25" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="J81" s="4"/>
     </row>
     <row r="82" spans="1:10" ht="132" customHeight="1">
       <c r="A82" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F82" s="25" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="G82" s="25" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J82" s="6"/>
     </row>
     <row r="83" spans="1:10" ht="158.4">
       <c r="A83" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F83" s="25" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="G83" s="25" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="H83" s="4"/>
       <c r="I83" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J83" s="4"/>
     </row>
     <row r="84" spans="1:10" ht="144">
       <c r="A84" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F84" s="25" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="G84" s="25" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J84" s="15"/>
     </row>
     <row r="85" spans="1:10" ht="172.8">
       <c r="A85" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F85" s="25" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G85" s="25" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J85" s="15"/>
     </row>
     <row r="86" spans="1:10" ht="172.8">
       <c r="A86" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F86" s="25" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G86" s="25" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="H86" s="4"/>
       <c r="I86" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J86" s="15"/>
     </row>
     <row r="87" spans="1:10" ht="201.6">
       <c r="A87" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="E87" s="13" t="s">
         <v>17</v>
       </c>
       <c r="F87" s="26" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G87" s="26" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="H87" s="13"/>
       <c r="I87" s="13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J87" s="14"/>
     </row>
     <row r="88" spans="1:10" ht="115.2">
       <c r="A88" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E88" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F88" s="25" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="G88" s="25" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="H88" s="4"/>
       <c r="I88" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J88" s="6"/>
     </row>
     <row r="89" spans="1:10" ht="104.4" customHeight="1">
       <c r="A89" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F89" s="25" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="G89" s="25" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="H89" s="4"/>
       <c r="I89" s="6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J89" s="4"/>
     </row>
     <row r="90" spans="1:10" ht="90.6" customHeight="1">
       <c r="A90" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E90" s="24" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="F90" s="25" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="G90" s="25" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="H90" s="4"/>
       <c r="I90" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J90" s="4"/>
     </row>
     <row r="91" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>24</v>
@@ -9591,720 +9586,720 @@
         <v>17</v>
       </c>
       <c r="F91" s="26" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="G91" s="26" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="H91" s="13"/>
       <c r="I91" s="13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J91" s="14"/>
     </row>
     <row r="92" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A92" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E92" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F92" s="25" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="G92" s="25" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="H92" s="4"/>
       <c r="I92" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J92" s="15"/>
     </row>
     <row r="93" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A93" s="4" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F93" s="25" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="G93" s="25" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="H93" s="4"/>
       <c r="I93" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="J93" s="15"/>
     </row>
     <row r="94" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A94" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E94" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F94" s="25" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="G94" s="25" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="H94" s="4"/>
       <c r="I94" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J94" s="4"/>
     </row>
     <row r="95" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A95" s="4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F95" s="25" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="G95" s="25" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="H95" s="4"/>
       <c r="I95" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J95" s="4"/>
     </row>
     <row r="96" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A96" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F96" s="25" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="G96" s="25" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="H96" s="4"/>
       <c r="I96" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J96" s="4"/>
     </row>
     <row r="97" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A97" s="4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F97" s="25" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="G97" s="25" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="H97" s="4"/>
       <c r="I97" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J97" s="4"/>
     </row>
     <row r="98" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A98" s="4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E98" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F98" s="25" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="G98" s="25" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="H98" s="4"/>
       <c r="I98" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J98" s="4"/>
     </row>
     <row r="99" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A99" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E99" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F99" s="25" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="G99" s="25" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="H99" s="4"/>
       <c r="I99" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J99" s="4"/>
     </row>
     <row r="100" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A100" s="4" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F100" s="25" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="G100" s="25" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="H100" s="4"/>
       <c r="I100" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J100" s="4"/>
     </row>
     <row r="101" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A101" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F101" s="25" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="G101" s="25" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="H101" s="4"/>
       <c r="I101" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J101" s="4"/>
     </row>
     <row r="102" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A102" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F102" s="25" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="G102" s="25" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="H102" s="4"/>
       <c r="I102" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J102" s="4"/>
     </row>
     <row r="103" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A103" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F103" s="25" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="G103" s="25" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="H103" s="4"/>
       <c r="I103" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J103" s="4"/>
     </row>
     <row r="104" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A104" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F104" s="25" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="G104" s="25" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="H104" s="4"/>
       <c r="I104" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J104" s="4"/>
     </row>
     <row r="105" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A105" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F105" s="25" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="G105" s="25" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="H105" s="4"/>
       <c r="I105" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J105" s="4"/>
     </row>
     <row r="106" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A106" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F106" s="25" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="G106" s="25" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="H106" s="4"/>
       <c r="I106" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J106" s="4"/>
     </row>
     <row r="107" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A107" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E107" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F107" s="25" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="G107" s="25" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="H107" s="4"/>
       <c r="I107" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="J107" s="4"/>
     </row>
     <row r="108" spans="1:10" ht="112.95" customHeight="1">
       <c r="A108" s="17" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B108" s="17" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C108" s="17" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D108" s="17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F108" s="27" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="G108" s="27" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
       <c r="H108" s="17"/>
       <c r="I108" s="17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J108" s="17"/>
     </row>
     <row r="109" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A109" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E109" s="21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F109" s="25" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="G109" s="25" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="H109" s="4"/>
       <c r="I109" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J109" s="4"/>
     </row>
     <row r="110" spans="1:10" ht="75.599999999999994" customHeight="1">
       <c r="A110" s="18" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B110" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C110" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D110" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="C110" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D110" s="20" t="s">
-        <v>213</v>
-      </c>
       <c r="E110" s="18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F110" s="28" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="G110" s="28" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="H110" s="18"/>
       <c r="I110" s="18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J110" s="18"/>
     </row>
     <row r="111" spans="1:10" ht="111" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E111" s="21" t="s">
         <v>17</v>
       </c>
       <c r="F111" s="25" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="G111" s="25" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="H111" s="4"/>
       <c r="I111" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J111" s="4"/>
     </row>
     <row r="112" spans="1:10" ht="142.94999999999999" customHeight="1">
       <c r="A112" s="18" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B112" s="18" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C112" s="19" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D112" s="20" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="E112" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F112" s="28" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="G112" s="28" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="H112" s="18"/>
       <c r="I112" s="18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J112" s="18"/>
     </row>
     <row r="113" spans="1:10" ht="144">
       <c r="A113" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E113" s="21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F113" s="25" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G113" s="25" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="H113" s="4"/>
       <c r="I113" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J113" s="4"/>
     </row>
     <row r="114" spans="1:10" ht="129.6">
       <c r="A114" s="18" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B114" s="18" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C114" s="19" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="D114" s="20" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E114" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F114" s="28" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="G114" s="28" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="H114" s="18"/>
       <c r="I114" s="18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J114" s="18"/>
     </row>
     <row r="115" spans="1:10" ht="151.05000000000001" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B115" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="D115" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="C115" s="5" t="s">
-        <v>461</v>
-      </c>
-      <c r="D115" s="6" t="s">
-        <v>213</v>
-      </c>
       <c r="E115" s="21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F115" s="25" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="G115" s="25" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="H115" s="4"/>
       <c r="I115" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J115" s="4"/>
     </row>
     <row r="116" spans="1:10" ht="151.05000000000001" customHeight="1">
       <c r="A116" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E116" s="21" t="s">
         <v>17</v>
       </c>
       <c r="F116" s="25" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G116" s="25" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="H116" s="4"/>
       <c r="I116" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J116" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E108 E109 E110 E111 E112 E113 E114 E115 E116 E2:E11 E13:E107">
       <formula1>"full match,partial match,skip"</formula1>
     </dataValidation>
@@ -10373,7 +10368,7 @@
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="72">
       <c r="A2" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>15</v>
@@ -10384,20 +10379,20 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="86.4">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -10408,20 +10403,20 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="6" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="86.4">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>15</v>
@@ -10434,36 +10429,36 @@
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="96.6" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -10471,49 +10466,49 @@
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="118.2" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="6" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="96.6" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -10521,27 +10516,27 @@
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="118.2" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J8" s="4"/>
     </row>

</xml_diff>